<commit_message>
Removing TWB PNPC table and adding two extra fields to TWB Episode instead.
</commit_message>
<xml_diff>
--- a/data/_orig/WAYBACK-3-0-twb-episodes-delete.xlsx
+++ b/data/_orig/WAYBACK-3-0-twb-episodes-delete.xlsx
@@ -12,26 +12,25 @@
     <sheet name="Clients" sheetId="3" r:id="rId3"/>
     <sheet name="Episodes" sheetId="4" r:id="rId4"/>
     <sheet name="TWB Episodes" sheetId="5" r:id="rId5"/>
-    <sheet name="TWB PNPCs" sheetId="6" r:id="rId6"/>
-    <sheet name="TWB Critical Incidents" sheetId="7" r:id="rId7"/>
-    <sheet name="TWB Recommendation Outs" sheetId="8" r:id="rId8"/>
-    <sheet name="Collection Occasions" sheetId="9" r:id="rId9"/>
-    <sheet name="K10+" sheetId="10" r:id="rId10"/>
-    <sheet name="K5" sheetId="11" r:id="rId11"/>
-    <sheet name="SDQ" sheetId="12" r:id="rId12"/>
-    <sheet name="WHO-5" sheetId="13" r:id="rId13"/>
-    <sheet name="SIDAS" sheetId="14" r:id="rId14"/>
-    <sheet name="TWB Plans" sheetId="15" r:id="rId15"/>
-    <sheet name="TWB NIs" sheetId="16" r:id="rId16"/>
-    <sheet name="Service Contacts" sheetId="17" r:id="rId17"/>
-    <sheet name="Practitioners" sheetId="18" r:id="rId18"/>
+    <sheet name="TWB Critical Incidents" sheetId="6" r:id="rId6"/>
+    <sheet name="TWB Recommendation Outs" sheetId="7" r:id="rId7"/>
+    <sheet name="Collection Occasions" sheetId="8" r:id="rId8"/>
+    <sheet name="K10+" sheetId="9" r:id="rId9"/>
+    <sheet name="K5" sheetId="10" r:id="rId10"/>
+    <sheet name="SDQ" sheetId="11" r:id="rId11"/>
+    <sheet name="WHO-5" sheetId="12" r:id="rId12"/>
+    <sheet name="SIDAS" sheetId="13" r:id="rId13"/>
+    <sheet name="TWB Plans" sheetId="14" r:id="rId14"/>
+    <sheet name="TWB NIs" sheetId="15" r:id="rId15"/>
+    <sheet name="Service Contacts" sheetId="16" r:id="rId16"/>
+    <sheet name="Practitioners" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="266">
   <si>
     <t>key</t>
   </si>
@@ -264,25 +263,16 @@
     <t>twb_primary_nominated_professional_consent_date</t>
   </si>
   <si>
+    <t>twb_primary_nominated_professional_contact_entry_date</t>
+  </si>
+  <si>
+    <t>twb_primary_nominated_professional_contact_exit_date</t>
+  </si>
+  <si>
     <t>twb_previous_suicide_attempts</t>
   </si>
   <si>
     <t>twb_method_of_suicide_attempt</t>
-  </si>
-  <si>
-    <t>twb_pnpc_key</t>
-  </si>
-  <si>
-    <t>twb_pnpc_reason</t>
-  </si>
-  <si>
-    <t>twb_pnpc_date</t>
-  </si>
-  <si>
-    <t>PNPC04-1</t>
-  </si>
-  <si>
-    <t>PNPC05-1</t>
   </si>
   <si>
     <t>twb_critical_incident_key</t>
@@ -1206,302 +1196,6 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I1" t="s">
-        <v>115</v>
-      </c>
-      <c r="J1" t="s">
-        <v>116</v>
-      </c>
-      <c r="K1" t="s">
-        <v>117</v>
-      </c>
-      <c r="L1" t="s">
-        <v>118</v>
-      </c>
-      <c r="M1" t="s">
-        <v>119</v>
-      </c>
-      <c r="N1" t="s">
-        <v>120</v>
-      </c>
-      <c r="O1" t="s">
-        <v>121</v>
-      </c>
-      <c r="P1" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>123</v>
-      </c>
-      <c r="R1" t="s">
-        <v>124</v>
-      </c>
-      <c r="S1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="I2">
-        <v>5</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2">
-        <v>4</v>
-      </c>
-      <c r="L2">
-        <v>5</v>
-      </c>
-      <c r="M2">
-        <v>4</v>
-      </c>
-      <c r="N2">
-        <v>3</v>
-      </c>
-      <c r="O2">
-        <v>3</v>
-      </c>
-      <c r="P2">
-        <v>5</v>
-      </c>
-      <c r="Q2">
-        <v>4</v>
-      </c>
-      <c r="R2">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3">
-        <v>3</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>3</v>
-      </c>
-      <c r="I3">
-        <v>4</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3">
-        <v>3</v>
-      </c>
-      <c r="L3">
-        <v>5</v>
-      </c>
-      <c r="M3">
-        <v>4</v>
-      </c>
-      <c r="N3">
-        <v>3</v>
-      </c>
-      <c r="O3">
-        <v>2</v>
-      </c>
-      <c r="P3">
-        <v>4</v>
-      </c>
-      <c r="Q3">
-        <v>4</v>
-      </c>
-      <c r="R3">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <v>4</v>
-      </c>
-      <c r="M4">
-        <v>4</v>
-      </c>
-      <c r="N4">
-        <v>4</v>
-      </c>
-      <c r="O4">
-        <v>3</v>
-      </c>
-      <c r="P4">
-        <v>2</v>
-      </c>
-      <c r="Q4">
-        <v>2</v>
-      </c>
-      <c r="R4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5">
-        <v>3</v>
-      </c>
-      <c r="L5">
-        <v>2</v>
-      </c>
-      <c r="M5">
-        <v>2</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>2</v>
-      </c>
-      <c r="P5">
-        <v>3</v>
-      </c>
-      <c r="Q5">
-        <v>2</v>
-      </c>
-      <c r="R5">
-        <v>99</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1513,31 +1207,31 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G1" t="s">
         <v>130</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>131</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>132</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>133</v>
-      </c>
-      <c r="H1" t="s">
-        <v>134</v>
-      </c>
-      <c r="I1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1545,10 +1239,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1569,7 +1263,7 @@
         <v>99</v>
       </c>
       <c r="J2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1577,10 +1271,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D3">
         <v>9</v>
@@ -1601,7 +1295,7 @@
         <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1609,10 +1303,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1638,10 +1332,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1667,7 +1361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BB4"/>
   <sheetViews>
@@ -1680,163 +1374,163 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" t="s">
+        <v>139</v>
+      </c>
+      <c r="F1" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" t="s">
         <v>141</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>142</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>143</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>144</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>145</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>146</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>147</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>148</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>149</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>150</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>151</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>152</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>153</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>154</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>155</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>156</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>157</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>158</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>159</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>160</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>161</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>162</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>163</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>164</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>165</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>166</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>167</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>168</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>169</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>170</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>171</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>172</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>173</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>174</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>175</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>176</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>177</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>178</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>179</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>180</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>181</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>182</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>183</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>184</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>185</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>186</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>187</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>188</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>189</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>190</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:54">
@@ -1844,13 +1538,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -2008,13 +1702,13 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E3">
         <v>9</v>
@@ -2169,13 +1863,13 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2330,7 +2024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -2343,28 +2037,28 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" t="s">
         <v>198</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>199</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>200</v>
-      </c>
-      <c r="G1" t="s">
-        <v>201</v>
-      </c>
-      <c r="H1" t="s">
-        <v>202</v>
-      </c>
-      <c r="I1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2372,10 +2066,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -2398,10 +2092,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -2424,10 +2118,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -2450,10 +2144,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -2476,7 +2170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -2489,28 +2183,28 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" t="s">
+        <v>207</v>
+      </c>
+      <c r="G1" t="s">
         <v>208</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>209</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>210</v>
-      </c>
-      <c r="G1" t="s">
-        <v>211</v>
-      </c>
-      <c r="H1" t="s">
-        <v>212</v>
-      </c>
-      <c r="I1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2518,10 +2212,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2539,7 +2233,7 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2547,28 +2241,114 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>9</v>
+      </c>
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" t="s">
         <v>215</v>
       </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>217</v>
+      </c>
       <c r="C3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D3">
-        <v>9</v>
-      </c>
-      <c r="E3">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>9</v>
-      </c>
-      <c r="G3">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>9</v>
-      </c>
-      <c r="I3" t="s">
-        <v>99</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2589,16 +2369,16 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2606,10 +2386,10 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2620,10 +2400,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -2634,10 +2414,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D4">
         <v>2</v>
@@ -2648,10 +2428,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2663,92 +2443,6 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D1" t="s">
-        <v>224</v>
-      </c>
-      <c r="E1" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>227</v>
-      </c>
-      <c r="C3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>228</v>
-      </c>
-      <c r="C4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R3"/>
   <sheetViews>
@@ -2761,55 +2455,55 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C1" t="s">
         <v>37</v>
       </c>
       <c r="D1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F1" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" t="s">
         <v>231</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>232</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>233</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>234</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>235</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>236</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>237</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>238</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>239</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>240</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>241</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>242</v>
-      </c>
-      <c r="P1" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>244</v>
-      </c>
-      <c r="R1" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -2817,13 +2511,13 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E2">
         <v>21052016</v>
@@ -2873,13 +2567,13 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C3" t="s">
         <v>66</v>
       </c>
       <c r="D3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E3">
         <v>15062016</v>
@@ -2926,7 +2620,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I13"/>
   <sheetViews>
@@ -2939,28 +2633,28 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" t="s">
         <v>250</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>251</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>252</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>253</v>
-      </c>
-      <c r="G1" t="s">
-        <v>254</v>
-      </c>
-      <c r="H1" t="s">
-        <v>255</v>
-      </c>
-      <c r="I1" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2968,7 +2662,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C2">
         <v>8</v>
@@ -2997,7 +2691,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3018,7 +2712,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3026,7 +2720,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -3052,7 +2746,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C5">
         <v>99</v>
@@ -3078,7 +2772,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -3107,7 +2801,7 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -3133,7 +2827,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -3162,7 +2856,7 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -3188,7 +2882,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -3209,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3217,7 +2911,7 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -3243,7 +2937,7 @@
         <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -3264,7 +2958,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3272,7 +2966,7 @@
         <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -3795,13 +3489,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -3841,8 +3535,14 @@
       <c r="M1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3877,13 +3577,19 @@
         <v>15042020</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>16042020</v>
       </c>
       <c r="M2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>9099999</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3915,9 +3621,15 @@
         <v>9099999</v>
       </c>
       <c r="L3">
-        <v>3</v>
+        <v>9099999</v>
       </c>
       <c r="M3">
+        <v>9099999</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
         <v>1</v>
       </c>
     </row>
@@ -3939,16 +3651,16 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
         <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3956,7 +3668,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
@@ -3973,7 +3685,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -4003,16 +3715,16 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
         <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4020,16 +3732,16 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>10032020</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4037,16 +3749,16 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>16032020</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4055,70 +3767,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -4131,19 +3779,19 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
         <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4151,7 +3799,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
@@ -4163,7 +3811,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4171,7 +3819,7 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -4183,7 +3831,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -4191,7 +3839,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -4203,7 +3851,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -4211,7 +3859,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
         <v>64</v>
@@ -4223,7 +3871,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -4231,7 +3879,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" t="s">
         <v>66</v>
@@ -4243,7 +3891,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -4251,7 +3899,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C7" t="s">
         <v>64</v>
@@ -4263,7 +3911,7 @@
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -4271,7 +3919,7 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
         <v>66</v>
@@ -4283,7 +3931,7 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -4291,7 +3939,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
         <v>66</v>
@@ -4303,7 +3951,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4311,7 +3959,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C10" t="s">
         <v>64</v>
@@ -4323,7 +3971,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -4331,7 +3979,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C11" t="s">
         <v>66</v>
@@ -4343,6 +3991,302 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M1" t="s">
+        <v>116</v>
+      </c>
+      <c r="N1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" t="s">
+        <v>118</v>
+      </c>
+      <c r="P1" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>120</v>
+      </c>
+      <c r="R1" t="s">
+        <v>121</v>
+      </c>
+      <c r="S1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <v>5</v>
+      </c>
+      <c r="M2">
+        <v>4</v>
+      </c>
+      <c r="N2">
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <v>3</v>
+      </c>
+      <c r="P2">
+        <v>5</v>
+      </c>
+      <c r="Q2">
+        <v>4</v>
+      </c>
+      <c r="R2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>3</v>
+      </c>
+      <c r="L3">
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>4</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
+      <c r="P4">
+        <v>2</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <v>3</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
         <v>99</v>
       </c>
     </row>

</xml_diff>